<commit_message>
All good to run models
</commit_message>
<xml_diff>
--- a/Result_files/RepWeeks.xlsx
+++ b/Result_files/RepWeeks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rolvur Reinert\Desktop\Thesis\Result_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1C75EDD-A76D-4AD7-B780-19FCB7B7DDEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54814EF1-D244-4C27-AE31-AEBF69EE7F8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -53,14 +53,21 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -90,12 +97,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -430,14 +439,14 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>43885</v>
       </c>
       <c r="C2">
         <v>0.13461538461538461</v>
       </c>
-      <c r="D2" s="2">
-        <v>43885</v>
+      <c r="D2" s="3">
+        <v>44249</v>
       </c>
       <c r="E2">
         <v>0.23076923076923081</v>
@@ -447,14 +456,14 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>44039</v>
       </c>
       <c r="C3">
         <v>3.8461538461538457E-2</v>
       </c>
-      <c r="D3" s="2">
-        <v>44039</v>
+      <c r="D3" s="3">
+        <v>44403</v>
       </c>
       <c r="E3">
         <v>3.8461538461538457E-2</v>
@@ -464,14 +473,14 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>43990</v>
       </c>
       <c r="C4">
         <v>5.7692307692307702E-2</v>
       </c>
-      <c r="D4" s="2">
-        <v>44060</v>
+      <c r="D4" s="3">
+        <v>44424</v>
       </c>
       <c r="E4">
         <v>5.7692307692307702E-2</v>
@@ -481,14 +490,14 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <v>43997</v>
       </c>
       <c r="C5">
         <v>5.7692307692307702E-2</v>
       </c>
-      <c r="D5" s="2">
-        <v>44011</v>
+      <c r="D5" s="3">
+        <v>44375</v>
       </c>
       <c r="E5">
         <v>3.8461538461538457E-2</v>
@@ -498,14 +507,14 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <v>44060</v>
       </c>
       <c r="C6">
         <v>7.6923076923076927E-2</v>
       </c>
-      <c r="D6" s="2">
-        <v>44095</v>
+      <c r="D6" s="3">
+        <v>44459</v>
       </c>
       <c r="E6">
         <v>0.1153846153846154</v>
@@ -515,14 +524,14 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <v>44053</v>
       </c>
       <c r="C7">
         <v>0.1730769230769231</v>
       </c>
-      <c r="D7" s="2">
-        <v>44053</v>
+      <c r="D7" s="3">
+        <v>44417</v>
       </c>
       <c r="E7">
         <v>1.9230769230769228E-2</v>
@@ -532,14 +541,14 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="3">
         <v>44004</v>
       </c>
       <c r="C8">
         <v>3.8461538461538457E-2</v>
       </c>
-      <c r="D8" s="2">
-        <v>44025</v>
+      <c r="D8" s="3">
+        <v>44389</v>
       </c>
       <c r="E8">
         <v>5.7692307692307702E-2</v>
@@ -549,14 +558,14 @@
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="3">
         <v>44074</v>
       </c>
       <c r="C9">
         <v>9.6153846153846159E-2</v>
       </c>
-      <c r="D9" s="2">
-        <v>43941</v>
+      <c r="D9" s="3">
+        <v>44305</v>
       </c>
       <c r="E9">
         <v>0.15384615384615391</v>
@@ -566,14 +575,14 @@
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="3">
         <v>43948</v>
       </c>
       <c r="C10">
         <v>0.21153846153846151</v>
       </c>
-      <c r="D10" s="2">
-        <v>43983</v>
+      <c r="D10" s="3">
+        <v>44347</v>
       </c>
       <c r="E10">
         <v>9.6153846153846159E-2</v>
@@ -583,18 +592,24 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="3">
         <v>43843</v>
       </c>
       <c r="C11">
         <v>0.1153846153846154</v>
       </c>
-      <c r="D11" s="2">
-        <v>44081</v>
+      <c r="D11" s="3">
+        <v>44445</v>
       </c>
       <c r="E11">
         <v>0.19230769230769229</v>
       </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>